<commit_message>
Risolti errori test 28 e 36
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.0/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.0/accreditamento-checklist_V8.2.6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20241210_docs\0_Accreditamento\docs_per_accreditamento\accreditamento_8.2.6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20241210_docs\0_Accreditamento\docs_per_accreditamento\A1#111#VITALSOFTWAREXX\VitalSoftware\Isolab9002\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCE0C40-2A39-4631-AC8B-9C7B50813A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277515DB-1A21-4257-BF45-2C3B1B94359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="184">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -654,12 +654,6 @@
     <t>12:00:52</t>
   </si>
   <si>
-    <t>12:01:44</t>
-  </si>
-  <si>
-    <t>12:01:51</t>
-  </si>
-  <si>
     <t>12:00:59</t>
   </si>
   <si>
@@ -708,18 +702,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.a2aea048da11324375f7e287c382a58f0c76be29f8bba948511b240dca9b6999.5b27a4ad42^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>1751f03ad7e60c747dbb226788ffa343</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.a2aea048da11324375f7e287c382a58f0c76be29f8bba948511b240dca9b6999.044fc3558e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c1f152a5a99c7769885adb4c5313ce49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.a2aea048da11324375f7e287c382a58f0c76be29f8bba948511b240dca9b6999.a27d730da3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>6bcef270bfd6f555165fac5bec468814</t>
   </si>
   <si>
@@ -808,6 +790,21 @@
   </si>
   <si>
     <t>L'errore segnalato sul monitor va in coda di retry. Dopo 5 tentativi il problema viene memorizzato in un file che sara' gestito dal supporto tecnico.</t>
+  </si>
+  <si>
+    <t>22:05:11</t>
+  </si>
+  <si>
+    <t>22:06:45</t>
+  </si>
+  <si>
+    <t>7068d3819883853c56c4e33b647628d8</t>
+  </si>
+  <si>
+    <t>c2f0c697ff2896fe9ada69a563bb5dd8</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +2889,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3204,10 +3201,10 @@
         <v>132</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J10" s="38" t="s">
         <v>50</v>
@@ -3247,16 +3244,16 @@
         <v>43</v>
       </c>
       <c r="F11" s="36">
-        <v>45753</v>
+        <v>45936</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="J11" s="38" t="s">
         <v>50</v>
@@ -3270,7 +3267,7 @@
         <v>50</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P11" s="38" t="s">
         <v>50</v>
@@ -3282,7 +3279,7 @@
         <v>50</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T11" s="38" t="s">
         <v>73</v>
@@ -3310,16 +3307,16 @@
         <v>48</v>
       </c>
       <c r="F12" s="36">
-        <v>45753</v>
+        <v>45936</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>50</v>
@@ -3333,7 +3330,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P12" s="38" t="s">
         <v>50</v>
@@ -3345,7 +3342,7 @@
         <v>50</v>
       </c>
       <c r="S12" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T12" s="38" t="s">
         <v>73</v>
@@ -3376,7 +3373,7 @@
         <v>45753</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="42"/>
@@ -3392,7 +3389,7 @@
         <v>50</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="P13" s="38" t="s">
         <v>50</v>
@@ -3404,7 +3401,7 @@
         <v>50</v>
       </c>
       <c r="S13" s="38" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="T13" s="38" t="s">
         <v>73</v>
@@ -3437,13 +3434,13 @@
         <v>45753</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J14" s="38" t="s">
         <v>50</v>
@@ -3457,7 +3454,7 @@
         <v>50</v>
       </c>
       <c r="O14" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P14" s="38" t="s">
         <v>50</v>
@@ -3469,7 +3466,7 @@
         <v>50</v>
       </c>
       <c r="S14" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T14" s="38" t="s">
         <v>73</v>
@@ -3500,13 +3497,13 @@
         <v>45753</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J15" s="38" t="s">
         <v>50</v>
@@ -3520,7 +3517,7 @@
         <v>50</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P15" s="38" t="s">
         <v>50</v>
@@ -3532,7 +3529,7 @@
         <v>50</v>
       </c>
       <c r="S15" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T15" s="38" t="s">
         <v>73</v>
@@ -3563,13 +3560,13 @@
         <v>45753</v>
       </c>
       <c r="G16" s="47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J16" s="38" t="s">
         <v>50</v>
@@ -3583,7 +3580,7 @@
         <v>50</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P16" s="38" t="s">
         <v>50</v>
@@ -3595,7 +3592,7 @@
         <v>50</v>
       </c>
       <c r="S16" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T16" s="38" t="s">
         <v>73</v>
@@ -3626,13 +3623,13 @@
         <v>45753</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J17" s="38" t="s">
         <v>50</v>
@@ -3646,7 +3643,7 @@
         <v>50</v>
       </c>
       <c r="O17" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P17" s="38" t="s">
         <v>50</v>
@@ -3658,7 +3655,7 @@
         <v>50</v>
       </c>
       <c r="S17" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T17" s="38" t="s">
         <v>73</v>
@@ -3689,13 +3686,13 @@
         <v>45753</v>
       </c>
       <c r="G18" s="47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>50</v>
@@ -3709,7 +3706,7 @@
         <v>50</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P18" s="38" t="s">
         <v>50</v>
@@ -3721,7 +3718,7 @@
         <v>50</v>
       </c>
       <c r="S18" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T18" s="38" t="s">
         <v>73</v>
@@ -3752,13 +3749,13 @@
         <v>45753</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>50</v>
@@ -3772,7 +3769,7 @@
         <v>50</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P19" s="38" t="s">
         <v>50</v>
@@ -3784,7 +3781,7 @@
         <v>50</v>
       </c>
       <c r="S19" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T19" s="38" t="s">
         <v>73</v>
@@ -3815,13 +3812,13 @@
         <v>45753</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I20" s="42" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>50</v>
@@ -3835,7 +3832,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P20" s="38" t="s">
         <v>50</v>
@@ -3847,7 +3844,7 @@
         <v>50</v>
       </c>
       <c r="S20" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T20" s="38" t="s">
         <v>73</v>
@@ -3878,13 +3875,13 @@
         <v>45753</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J21" s="38" t="s">
         <v>50</v>
@@ -3898,7 +3895,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P21" s="38" t="s">
         <v>50</v>
@@ -3910,7 +3907,7 @@
         <v>50</v>
       </c>
       <c r="S21" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T21" s="38" t="s">
         <v>73</v>
@@ -3941,13 +3938,13 @@
         <v>45753</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I22" s="42" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J22" s="38" t="s">
         <v>50</v>
@@ -3990,13 +3987,13 @@
         <v>45753</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I23" s="42" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J23" s="38" t="s">
         <v>50</v>
@@ -4039,13 +4036,13 @@
         <v>45753</v>
       </c>
       <c r="G24" s="47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J24" s="38" t="s">
         <v>50</v>
@@ -4088,13 +4085,13 @@
         <v>45753</v>
       </c>
       <c r="G25" s="48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J25" s="38" t="s">
         <v>50</v>
@@ -4108,7 +4105,7 @@
         <v>50</v>
       </c>
       <c r="O25" s="35" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P25" s="38" t="s">
         <v>50</v>
@@ -4120,7 +4117,7 @@
         <v>50</v>
       </c>
       <c r="S25" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T25" s="38" t="s">
         <v>73</v>
@@ -4151,13 +4148,13 @@
         <v>45753</v>
       </c>
       <c r="G26" s="47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="J26" s="38" t="s">
         <v>50</v>
@@ -4171,7 +4168,7 @@
         <v>50</v>
       </c>
       <c r="O26" s="38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P26" s="38" t="s">
         <v>50</v>
@@ -4183,7 +4180,7 @@
         <v>50</v>
       </c>
       <c r="S26" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T26" s="38" t="s">
         <v>73</v>
@@ -10489,15 +10486,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10755,6 +10743,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10768,14 +10765,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10790,6 +10779,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>